<commit_message>
Addition of the step for Normalization (Library) and Normalization (Genotyping) and introduced changed done to master.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Normalization_planning_v4_5_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Normalization_planning_v4_5_0.xlsx
@@ -144,10 +144,10 @@
     <t xml:space="preserve">Source Container Coord</t>
   </si>
   <si>
-    <t xml:space="preserve">Source Container Location Barcode</t>
+    <t xml:space="preserve">Source Parent Container Barcode</t>
   </si>
   <si>
-    <t xml:space="preserve">Source Container Location Coord</t>
+    <t xml:space="preserve">Source Parent Container Coord</t>
   </si>
   <si>
     <t xml:space="preserve">Destination Container Barcode</t>
@@ -683,7 +683,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="24.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.86"/>
@@ -8262,7 +8262,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.74"/>

</xml_diff>